<commit_message>
one excel sheet can draw multiple chart on one upload
</commit_message>
<xml_diff>
--- a/my-server-express/upload/grapdata.xlsx
+++ b/my-server-express/upload/grapdata.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
   <si>
     <t>jan</t>
   </si>
@@ -51,13 +52,61 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Counts</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>Jamshedpur</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Grapes</t>
+  </si>
+  <si>
+    <t>pineapple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rourkela   </t>
+  </si>
+  <si>
+    <t>WaterMelon</t>
+  </si>
+  <si>
+    <t>Howrah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CKP </t>
+  </si>
+  <si>
+    <t>GNICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranchi </t>
+  </si>
+  <si>
+    <t>iWealth</t>
+  </si>
+  <si>
+    <t>Prepaid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,16 +114,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -82,14 +157,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,4 +570,352 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7">
+        <v>9219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7">
+        <v>27841</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7">
+        <v>25358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7">
+        <v>527723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7">
+        <v>29327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="7">
+        <v>45707</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="7">
+        <v>22930</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="7">
+        <v>110534</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="7">
+        <v>152629</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="7">
+        <v>107917</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="7">
+        <v>38567</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="7">
+        <v>129363</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="7">
+        <v>89924</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="7">
+        <v>640017</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="7">
+        <v>17756</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>